<commit_message>
Update logs, create new functions, improved performance
</commit_message>
<xml_diff>
--- a/locators.xlsx
+++ b/locators.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mirgo\OneDrive\Documents\vlad_workspace\workspace_python\letskodeit_project_aoutomation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20C87D80-8E3F-41E0-A257-4CF7132CD588}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{762FF9D5-CD44-411D-B071-6EDF8B1A17D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-870" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="39">
   <si>
     <t>page name</t>
   </si>
@@ -119,6 +119,24 @@
   </si>
   <si>
     <t>forgot password link 2</t>
+  </si>
+  <si>
+    <t>all courses link</t>
+  </si>
+  <si>
+    <t>header</t>
+  </si>
+  <si>
+    <t>//a[contains(@href,'/courses') and contains(text(),'ALL COURSES')]</t>
+  </si>
+  <si>
+    <t>all courses</t>
+  </si>
+  <si>
+    <t>selenium webdriver 4 with java</t>
+  </si>
+  <si>
+    <t>//a[@href='/courses/selenium-webdriver-with-java']</t>
   </si>
 </sst>
 </file>
@@ -460,10 +478,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:D11"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -671,6 +689,36 @@
       </c>
       <c r="E13" s="1"/>
     </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>